<commit_message>
Updates with the disposition of further CRs.
</commit_message>
<xml_diff>
--- a/Product/trunk/ProductDescriptions/MTOSI_R2-0_ProblemsAndFixes.xlsx
+++ b/Product/trunk/ProductDescriptions/MTOSI_R2-0_ProblemsAndFixes.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="-15" windowWidth="18210" windowHeight="8490"/>
+    <workbookView xWindow="45" yWindow="180" windowWidth="19320" windowHeight="12120" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>top of p 10</t>
   </si>
@@ -130,13 +134,151 @@
   </si>
   <si>
     <t>reference (e.g. CR)</t>
+  </si>
+  <si>
+    <t>artf1440</t>
+  </si>
+  <si>
+    <t>artf1283</t>
+  </si>
+  <si>
+    <t>artf1278</t>
+  </si>
+  <si>
+    <t>artf1246</t>
+  </si>
+  <si>
+    <t>artf1338</t>
+  </si>
+  <si>
+    <t>artf1670</t>
+  </si>
+  <si>
+    <t>artf1951</t>
+  </si>
+  <si>
+    <t>section 3.1.9.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FlowPoint hyperlink goes to goes to 3.1.6 Floating Termination Point (FTP). It should go to 3.1.9.3  Flow Point (FP)
+</t>
+  </si>
+  <si>
+    <t>fix the hyperlink</t>
+  </si>
+  <si>
+    <t>Proposed enhancements to the MTOSI R2.0 NMS-EMS Activation Interface to facilitate enhanced equipment, and protection group provisioning.</t>
+  </si>
+  <si>
+    <t>Problem with PMLocationType in PmDefintions.xsd.</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>artf1965</t>
+  </si>
+  <si>
+    <t>Missing supporting document SD1-33</t>
+  </si>
+  <si>
+    <t>FMW/SD/SD1-16_LayeredParameters.doc</t>
+  </si>
+  <si>
+    <t>No explicit string value for groups of layered tarnsmission parameters.</t>
+  </si>
+  <si>
+    <t>Update document to include explicit string for each grouping.</t>
+  </si>
+  <si>
+    <t>Needs to be added to the MTOSI package.</t>
+  </si>
+  <si>
+    <t>artf1974</t>
+  </si>
+  <si>
+    <t>FMW/SD1/SD1-33_ProbableCauses</t>
+  </si>
+  <si>
+    <t>Not being done as part of MTOSI R2.1.</t>
+  </si>
+  <si>
+    <t>Refer to the enclosed file.</t>
+  </si>
+  <si>
+    <t>Refer to Huawei comments in enclosed file.</t>
+  </si>
+  <si>
+    <t>Refer to Nortel comments in enclosed file.</t>
+  </si>
+  <si>
+    <t>MRI/IIS/wsdl/OperationsSystemRetrieval/OperationsSystemRetrievalMessages.xsd
+MRI/IIS/wsdl/ManagementDomainRetrieval/ManagementDomainRetrievalMessages.xsd</t>
+  </si>
+  <si>
+    <t>FMW/BA/TMF518_FMW
+FMW/SD/SD2-2_XML_ImplementationUserGuide
+FMW/SD/SD2-5_Communication_Styles
+FMW/SD/SD2-7_ObjectNaming
+FMW/SD/SD2-16_UsingHTTPAsMTOSITransport</t>
+  </si>
+  <si>
+    <t>FMW/BA/TMF518_NRF</t>
+  </si>
+  <si>
+    <t>The TCProfile MO has a boolean attribute (defaultProfile) to mark it as default. No mention in TMF doc on how to set/
+modify it. My proposal is to use the additionalInfo in TCProfileCreateData and TCProfileModifyData adding an specific 
+parameter name in SD1-1 and use case in TMF513</t>
+  </si>
+  <si>
+    <t>The operation getManagedElementsIterator is missing in ManagedElementRetrievalJms.wsdl description.
+Define the operation as done in ManagedElementRetrievalHttp.wsdl file</t>
+  </si>
+  <si>
+    <t>artf1997</t>
+  </si>
+  <si>
+    <t>The structure getManagedElementsIteratorRequest to be used as input is of type GetAllDataIteratorRequestType (in 
+MessageDefinitions.xsd in Framework pacakage) is empty.
+Define a type for getManagedElementsIteratorRequest.</t>
+  </si>
+  <si>
+    <t>artf1998</t>
+  </si>
+  <si>
+    <t>SD1-44 gives some example how it is possible to name the member of a LAG.
+The string used is lag_fragment=XXX and it seems related to LR_LAG_FRAGMENT (30) layer.
+But SD1-17 states that this layer is NOT used for naming, but just to highlight the aggreagation/fragmentation at LAG. 
+In addition it seems client of the LR_Ethernet. So it conflicts the general rule to use the more server LR for naming.
+Define clear rules in LAG member naming.</t>
+  </si>
+  <si>
+    <t>artf1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the example table of SD1-44 v1.1 paragraph 9.2.10 page 39, the Traffic Mapping Table is reported with additional 
+columns "Inner VLAN ID" and "Inner Priority" and it is stated "..In order to accommodate this
+situation, two more columns would be used: InnerVID and InnerPriority..".
+So it needs to add in SD1-16 the following layered paramters (missing in v3.3) valid for CPTP and FP:
+TrafficMappingFrom_Table_InnerVID
+TrafficMappingFrom_Table_InnerPriority
+</t>
+  </si>
+  <si>
+    <t>artf2005</t>
+  </si>
+  <si>
+    <t>Bernd</t>
+  </si>
+  <si>
+    <t>Michel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,18 +289,54 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.8000000000000007"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -170,9 +348,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -185,7 +361,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -222,30 +400,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -264,19 +446,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <oleLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" progId="Excel.Sheet.8">
+    <oleItems>
+      <oleItem name="'" icon="1" preferPic="1"/>
+    </oleItems>
+  </oleLink>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <oleLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" progId="Excel.Sheet.8">
+    <oleItems>
+      <oleItem name="'" icon="1" preferPic="1"/>
+    </oleItems>
+  </oleLink>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,16 +788,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="73.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="60" customWidth="1"/>
     <col min="5" max="5" width="46.140625" style="6" customWidth="1"/>
@@ -605,157 +832,392 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" ht="45">
+      <c r="A5" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="78" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="63.75" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="3">
-        <v>40175</v>
-      </c>
-      <c r="G2" s="2">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="60">
-      <c r="B3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30">
-      <c r="B4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="3">
-        <v>40175</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45">
-      <c r="B6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="3">
-        <v>40175</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="B9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="B10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="F10" s="3">
         <v>40175</v>
       </c>
       <c r="G10" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60">
+      <c r="A11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3">
+        <v>40175</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45">
+      <c r="A14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="3">
+        <v>40175</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30">
+      <c r="A17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="3">
+        <v>40175</v>
+      </c>
+      <c r="G18" s="2">
         <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
-      <c r="B11" t="s">
+    <row r="19" spans="1:7" ht="45">
+      <c r="A19" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="20" spans="1:7" ht="30">
+      <c r="A20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45">
+      <c r="A21" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75">
+      <c r="A23" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75">
+      <c r="A24" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="75">
+      <c r="A25" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="150">
+      <c r="A26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="165">
+      <c r="A27" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A7" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A8" r:id="rId5"/>
+    <hyperlink ref="A20" r:id="rId6"/>
+    <hyperlink ref="A21" r:id="rId7"/>
+    <hyperlink ref="A22" r:id="rId8"/>
+    <hyperlink ref="A23" r:id="rId9"/>
+    <hyperlink ref="A24" r:id="rId10"/>
+    <hyperlink ref="A25" r:id="rId11"/>
+    <hyperlink ref="A26" r:id="rId12"/>
+    <hyperlink ref="A27" r:id="rId13"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
+  <oleObjects>
+    <oleObject progId="Excel.Sheet.8" dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1025"/>
+    <oleObject progId="Excel.Sheet.8" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1026"/>
+  </oleObjects>
 </worksheet>
 </file>
 
@@ -767,6 +1229,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -779,6 +1242,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>